<commit_message>
params hotfix: grandiozo cheese
</commit_message>
<xml_diff>
--- a/app/data/params.xlsx
+++ b/app/data/params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mi\Desktop\code\git\2020.10-umalat\umalat\app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8159A11B-F480-4CBE-8256-4255CBCC3C8E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85225932-14D6-460A-9B26-C302B7C858E9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -774,11 +774,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="75.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
@@ -1633,8 +1636,11 @@
       <c r="P13">
         <v>840</v>
       </c>
-      <c r="S13">
-        <v>90</v>
+      <c r="Q13">
+        <v>25</v>
+      </c>
+      <c r="R13">
+        <v>50</v>
       </c>
       <c r="T13">
         <v>40</v>

</xml_diff>

<commit_message>
added enums for line names
</commit_message>
<xml_diff>
--- a/app/data/params.xlsx
+++ b/app/data/params.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mi\Desktop\code\git\2020.10-umalat\umalat\app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8BA55D8-ADC3-4AAD-AEC7-156E382B0916}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E50661-0CBA-4E78-B825-EC3A452A7229}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
@@ -774,13 +774,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="75.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.3">
@@ -1498,7 +1499,7 @@
         <v>25</v>
       </c>
       <c r="R11">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="T11">
         <v>40</v>
@@ -1566,7 +1567,7 @@
         <v>25</v>
       </c>
       <c r="R12">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="T12">
         <v>40</v>
@@ -2698,7 +2699,7 @@
         <v>25</v>
       </c>
       <c r="R29">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="T29">
         <v>40</v>
@@ -2766,7 +2767,7 @@
         <v>25</v>
       </c>
       <c r="R30">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="T30">
         <v>40</v>
@@ -2834,7 +2835,7 @@
         <v>25</v>
       </c>
       <c r="R31">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="T31">
         <v>40</v>
@@ -2902,7 +2903,7 @@
         <v>25</v>
       </c>
       <c r="R32">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="T32">
         <v>40</v>
@@ -2970,7 +2971,7 @@
         <v>25</v>
       </c>
       <c r="R33">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="T33">
         <v>40</v>
@@ -3629,7 +3630,7 @@
         <v>25</v>
       </c>
       <c r="R43">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="T43">
         <v>40</v>
@@ -4080,12 +4081,6 @@
       <c r="N50" t="s">
         <v>115</v>
       </c>
-      <c r="Q50">
-        <v>20</v>
-      </c>
-      <c r="R50">
-        <v>20</v>
-      </c>
       <c r="S50">
         <v>120</v>
       </c>
@@ -4359,7 +4354,7 @@
         <v>25</v>
       </c>
       <c r="R54">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="T54">
         <v>40</v>
@@ -4427,7 +4422,7 @@
         <v>25</v>
       </c>
       <c r="R55">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="T55">
         <v>40</v>
@@ -4621,12 +4616,6 @@
       <c r="P58">
         <v>850</v>
       </c>
-      <c r="Q58">
-        <v>20</v>
-      </c>
-      <c r="R58">
-        <v>20</v>
-      </c>
       <c r="S58">
         <v>120</v>
       </c>
@@ -4691,12 +4680,6 @@
       </c>
       <c r="P59">
         <v>850</v>
-      </c>
-      <c r="Q59">
-        <v>20</v>
-      </c>
-      <c r="R59">
-        <v>20</v>
       </c>
       <c r="S59">
         <v>120</v>

</xml_diff>